<commit_message>
update auto code generator
</commit_message>
<xml_diff>
--- a/xlsx/TestExcelData.xlsx
+++ b/xlsx/TestExcelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DerbyMasters_Server\DerbyWebServer\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DerbyMasters_Server\DerbyTornado-Doc\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7FC1B1-0C54-4D3C-B901-0B22FC03DB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3544B11-7F0F-495D-AC2F-F454048E503E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="1890" windowWidth="22905" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5430" yWindow="1755" windowWidth="22905" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,6 +107,38 @@
   </si>
   <si>
     <t>[int]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닉네임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스피드 범위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MinSpeed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -154,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,8 +199,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -191,11 +229,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -206,20 +255,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -500,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -513,125 +563,162 @@
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="E1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="str">
-        <f>IF(ISNUMBER(A5), "int", "string")</f>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="str">
+        <f>IF(ISNUMBER(A6), "int", "string")</f>
         <v>int</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="8" t="str">
-        <f>IF(ISNUMBER(C5), "int", "string")</f>
+      <c r="C3" s="5" t="str">
+        <f>IF(ISNUMBER(C6), "int", "string")</f>
         <v>string</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="E5" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D6" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="E6">
+        <v>50.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="E7">
+        <v>50.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D8" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3" t="s">
+      <c r="E8">
+        <v>50.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3">
+      <c r="C9" s="6"/>
+      <c r="D9" s="3">
         <v>250</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5" t="s">
+      <c r="E9">
+        <v>50.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5">
+      <c r="C10" s="6"/>
+      <c r="D10" s="3">
         <v>13</v>
+      </c>
+      <c r="E10">
+        <v>50.05</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>